<commit_message>
further update to Bacillus Data (addes "ts" in offline sheet)
</commit_message>
<xml_diff>
--- a/BacillusDaten/Stamm186/F6/offline_6.xlsx
+++ b/BacillusDaten/Stamm186/F6/offline_6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\biomoni\BacillusDaten\offline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\biomoni\BacillusDaten\Stamm186\F6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2616ADC-8BCC-483C-9B3E-0E04287C8250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED30727-690E-466C-97DB-CA05BB9392B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7890" yWindow="9315" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auswertunf" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Glucose [g/L]</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>SampleVolume [g]</t>
+  </si>
+  <si>
+    <t>ts</t>
   </si>
 </sst>
 </file>
@@ -562,7 +565,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -571,6 +574,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -671,7 +675,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Auswertunf!$B$1</c:f>
+              <c:f>Auswertunf!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -704,7 +708,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Auswertunf!$A$2:$A$26</c:f>
+              <c:f>Auswertunf!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="25"/>
@@ -773,7 +777,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Auswertunf!$B$2:$B$25</c:f>
+              <c:f>Auswertunf!$C$2:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -852,7 +856,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Auswertunf!$C$1</c:f>
+              <c:f>Auswertunf!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -889,7 +893,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Auswertunf!$A$2:$A$26</c:f>
+              <c:f>Auswertunf!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="25"/>
@@ -958,7 +962,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Auswertunf!$C$2:$C$25</c:f>
+              <c:f>Auswertunf!$D$2:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1037,7 +1041,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Auswertunf!$D$1</c:f>
+              <c:f>Auswertunf!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1073,7 +1077,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Auswertunf!$A$2:$A$26</c:f>
+              <c:f>Auswertunf!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1142,7 +1146,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Auswertunf!$D$2:$D$25</c:f>
+              <c:f>Auswertunf!$E$2:$E$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1457,7 +1461,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Auswertunf!$E$1</c:f>
+              <c:f>Auswertunf!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1477,7 +1481,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Auswertunf!$A$2:$A$26</c:f>
+              <c:f>Auswertunf!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1546,7 +1550,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Auswertunf!$E$2:$E$26</c:f>
+              <c:f>Auswertunf!$F$2:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1613,7 +1617,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Auswertunf!$F$1</c:f>
+              <c:f>Auswertunf!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1640,7 +1644,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Auswertunf!$A$2:$A$26</c:f>
+              <c:f>Auswertunf!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1709,7 +1713,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Auswertunf!$F$2:$F$26</c:f>
+              <c:f>Auswertunf!$G$2:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1737,7 +1741,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Auswertunf!$G$1</c:f>
+              <c:f>Auswertunf!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1773,7 +1777,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Auswertunf!$A$2:$A$26</c:f>
+              <c:f>Auswertunf!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1842,7 +1846,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Auswertunf!$G$2:$G$26</c:f>
+              <c:f>Auswertunf!$H$2:$H$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -2128,7 +2132,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Auswertunf!$H$1</c:f>
+              <c:f>Auswertunf!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2162,7 +2166,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Auswertunf!$I$2:$I$3</c:f>
+                <c:f>Auswertunf!$J$2:$J$3</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -2177,7 +2181,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Auswertunf!$I$2:$I$3</c:f>
+                <c:f>Auswertunf!$J$2:$J$3</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -2200,7 +2204,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Auswertunf!$A$2:$A$25</c:f>
+              <c:f>Auswertunf!$B$2:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="24"/>
@@ -2269,7 +2273,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Auswertunf!$H$2:$H$25</c:f>
+              <c:f>Auswertunf!$I$2:$I$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -2362,7 +2366,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Auswertunf!$J$1</c:f>
+              <c:f>Auswertunf!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2394,7 +2398,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Auswertunf!$A$2:$A$25</c:f>
+              <c:f>Auswertunf!$B$2:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="24"/>
@@ -2463,7 +2467,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Auswertunf!$J$2:$J$24</c:f>
+              <c:f>Auswertunf!$K$2:$K$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
@@ -2788,7 +2792,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Auswertunf!$K$1</c:f>
+              <c:f>Auswertunf!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2827,7 +2831,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Auswertunf!$L$2:$L$7</c:f>
+                <c:f>Auswertunf!$M$2:$M$7</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -2854,7 +2858,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Auswertunf!$L$2:$L$7</c:f>
+                <c:f>Auswertunf!$M$2:$M$7</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -2915,7 +2919,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Auswertunf!$A$2:$A$25</c:f>
+              <c:f>Auswertunf!$B$2:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="24"/>
@@ -2984,7 +2988,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Auswertunf!$K$2:$K$25</c:f>
+              <c:f>Auswertunf!$L$2:$L$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -3906,13 +3910,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>179294</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>146796</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>257735</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>32496</xdr:rowOff>
@@ -3942,13 +3946,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>212911</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>113177</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>291352</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>189377</xdr:rowOff>
@@ -3978,13 +3982,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>179293</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>134471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>638735</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>20171</xdr:rowOff>
@@ -4016,13 +4020,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>235324</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>11206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>336175</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>87406</xdr:rowOff>
@@ -4352,808 +4356,874 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="C24" sqref="C24:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>44579.689583333333</v>
+      </c>
+      <c r="B2" s="1">
         <v>9.9999999976716936E-2</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>24.710294634452463</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3">
         <v>6.8065688631790744</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>167780</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.13200000000000001</v>
       </c>
-      <c r="I2" t="e">
+      <c r="J2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>4.8430800000000003E-2</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>8.4942528735632177</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1.3285188543686643</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>2.5099999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>44580.327777777777</v>
+      </c>
+      <c r="B3" s="1">
         <v>15.416666666627862</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>24.028056479447759</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1.2045591983147759</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>7.7466586267605635</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>83962</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>2.8814999999999995</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.12037753112603691</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>1.0572223499999998</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>90.114942528735625</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>1.7604227863899824</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>1.7399999999999984</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>44580.379861111112</v>
+      </c>
+      <c r="B4" s="1">
         <v>16.666666666686069</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>24.112200502039535</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>2.0191176725850135</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>8.6823181841046271</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>4.9683333333333337</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>8.8821919216674039E-2</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1.8228815000000003</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>150.04597701149427</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>3.7254680468437775</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>2.0299999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>44580.426388888889</v>
+      </c>
+      <c r="B5" s="1">
         <v>17.783333333325572</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>20.891815186695951</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>2.9283398802287088</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>8.5533991825955731</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>124750</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>6.9710000000000001</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.24575801105965989</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>2.5576599</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>210.44827586206895</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>3.6925544522562435</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>2.3699999999999992</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>44580.486111111109</v>
+      </c>
+      <c r="B6" s="1">
         <v>19.21666666661622</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>17.98706871666144</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>4.0908070616912431</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>8.4940344190140831</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>65443</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>9.4333333333333336</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.32364383716260287</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>3.46109</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>296.02298850574709</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>9.8348632061956991</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>3.7399999999999984</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>44580.53125</v>
+      </c>
+      <c r="B7" s="1">
         <v>20.299999999988358</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>17.563583307185443</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>5.4424284917243444</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>9.3672280684104621</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>163920</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>161120</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>13.566666666666668</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.29224704161605009</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>4.9776100000000003</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>423.16091954022994</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>6.5297574884301275</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>3.3400000000000016</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>44580.570833333331</v>
+      </c>
+      <c r="B8" s="1">
         <v>21.249999999941792</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>17.288238782554128</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>7.3273020776406863</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>10.614774144869214</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>298530</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>225020</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>15.584999999999999</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.36314597615834765</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>5.7181365</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>512.64367816091954</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>17.220964925828536</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>3.2999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>44580.618750000001</v>
+      </c>
+      <c r="B9" s="1">
         <v>22.400000000023283</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>10.31100062754942</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>6.3370137634667465</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>7.9172215669014081</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>360270</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>145630</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>18.724999999999998</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.29012928152808087</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>6.8702024999999995</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>619.08045977011489</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>7.7343169792781454</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>3.3099999999999987</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>44580.657638888886</v>
+      </c>
+      <c r="B10" s="1">
         <v>23.333333333255723</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>7.2320404769375592</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>6.2700649383087566</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="3">
         <v>7.1999711770623742</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>492430</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>184350</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>21.77</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.68853104505170937</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>7.9874130000000001</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>745.74712643678151</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>9.7415064583299884</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>3.1099999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>44581.325694444444</v>
+      </c>
+      <c r="B11" s="1">
         <v>39.366666666639503</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>6.3301587700031376</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>11.34059400541679</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>7.6150815015090529</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>2804700</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>467780</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>43.430000000000007</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.95388678573508234</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>15.934467000000003</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>1957.816091954023</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>63.025515597492443</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>3.4299999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>44581.374305555553</v>
+      </c>
+      <c r="B12" s="1">
         <v>40.533333333267365</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>8.2093752745528707</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>11.840328444176949</v>
       </c>
-      <c r="D12" s="3">
+      <c r="E12" s="3">
         <v>7.8538696177062377</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>3125700</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>466830</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>46.353333333333332</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.45610671265980796</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>17.007037999999998</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>2148.5057471264367</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>4.3798985938522792</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>3.0700000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>44581.40347222222</v>
+      </c>
+      <c r="B13" s="1">
         <v>41.233333333279006</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>8.5901961091935988</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>11.305950370147457</v>
       </c>
-      <c r="D13" s="3">
+      <c r="E13" s="3">
         <v>7.7852014210261569</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>3125600</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>507500</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>46.776666666666664</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>1.2722552154867877</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>17.162358999999999</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>2120.4597701149428</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>88.46446268051578</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>3.5600000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>44581.443749999999</v>
+      </c>
+      <c r="B14" s="1">
         <v>42.199999999953434</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>10.865245058048323</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>10.948254835991573</v>
       </c>
-      <c r="D14" s="3">
+      <c r="E14" s="3">
         <v>8.6233964411468804</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>3543800</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>593590</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>46.866666666666674</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>1.3558883926538072</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>17.195380000000004</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>2196.5517241379312</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>15.517241379310462</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>3.2199999999999989</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>44581.479861111111</v>
+      </c>
+      <c r="B15" s="2">
         <v>43.066666666651145</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>13.207451208032634</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>12.577371784532049</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E15" s="3">
         <v>9.4053278420523139</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>4043100</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>775140</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>44.766666666666673</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>0.89074874871275345</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>16.424890000000001</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>2364.4827586206898</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>96.053517583637827</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>2.4300000000000015</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>44581.537499999999</v>
+      </c>
+      <c r="B16" s="2">
         <v>44.449999999953434</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>13.490301537496078</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>10.828734294312367</v>
       </c>
-      <c r="D16" s="3">
+      <c r="E16" s="3">
         <v>8.8484509180080479</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>3463800</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>778710</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>48.21</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>0.78479296632933437</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>17.688248999999999</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>2308.9655172413791</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>28.668427159760682</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>2.99</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>44581.572916666664</v>
+      </c>
+      <c r="B17" s="2">
         <v>45.299999999930151</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>14.228240665202385</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>12.307151429431237</v>
       </c>
-      <c r="D17" s="3">
+      <c r="E17" s="3">
         <v>8.7133296277665995</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>3312300</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>807390</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>47.23</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>3.2266546143025607</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>17.328686999999999</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>2348.2758620689651</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>49.198087798653276</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>2.5099999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>44581.604861111111</v>
+      </c>
+      <c r="B18" s="2">
         <v>46.066666666651145</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>15.584816128020083</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>12.503754059584713</v>
       </c>
-      <c r="D18" s="3">
+      <c r="E18" s="3">
         <v>8.952560764587524</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>2905500</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>930150</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>46.829999999999991</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>1.0289314845994362</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>17.181926999999998</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>2390.1149425287354</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>4.3798985938522792</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>3.49</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>44581.661805555559</v>
+      </c>
+      <c r="B19" s="2">
         <v>47.433333333407063</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>17.540275807969877</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>12.920343773698464</v>
       </c>
-      <c r="D19" s="3">
+      <c r="E19" s="3">
         <v>9.0571136317907435</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>2793700</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>1125700</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>45.433333333333337</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>0.36143233576056105</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>16.669490000000003</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>2337.9310344827586</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>63.762341138351765</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>2.5500000000000007</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>44582.330555555556</v>
+      </c>
+      <c r="B20" s="2">
         <v>63.483333333337214</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>23.331201757138377</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>20.640677893469753</v>
       </c>
-      <c r="D20" s="3">
+      <c r="E20" s="3">
         <v>8.6654834004024135</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>1557000</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>1930100</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>38.583333333333336</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>0.48013886880082146</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>14.156225000000001</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>2162.7586206896549</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>96.755941664192406</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>2.7899999999999991</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>44582.364583333336</v>
+      </c>
+      <c r="B21" s="2">
         <v>64.300000000046566</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>26.683926262943206</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>21.060731971110442</v>
       </c>
-      <c r="D21" s="3">
+      <c r="E21" s="3">
         <v>8.9875593938631777</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>1665200</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>1933800</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>38.220000000000006</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>1.5420440979427272</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>14.022918000000002</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>2263.4482758620688</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>30.344827586206975</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>3.26</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>